<commit_message>
refactor: update uc details
</commit_message>
<xml_diff>
--- a/1-exercices/ressources/uc_details.xlsx
+++ b/1-exercices/ressources/uc_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\formations\coderbase\m2i\poe-front-28112022\7-uml\1-exercices\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A166514F-8EFE-4A38-B6AD-1DD127B4710E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A575FBD-3F64-4BBC-A2C5-92487A24AC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Nom UC</t>
   </si>
@@ -107,34 +107,47 @@
     <t>Exécute le cas d'utilisation "Recevoir un cadeau"</t>
   </si>
   <si>
-    <t>Dans le cadre d'une méthode classique, on aurait directement une dépendance vers le  compte donc on aurait implémenter la partie compte en premier.
+    <t>Description courte</t>
+  </si>
+  <si>
+    <t>Acteur principal : client
+Acteur secondaire : Banque (système externe à notre périmètre fonctionnel avec lequel notre système doit communiquer pour la partie paiement)</t>
+  </si>
+  <si>
+    <t>Dans le cadre d'une méthode classique, on aurait directement une dépendance vers le  compte donc on aurait implémenté la partie compte en premier.
 Avec la méthode agile SCRUM,  on peut s'abstraire de cette dépendance d'un point de vue technique en demandant par exemple uniquement l'email.
 Réalisation du  cas d'utilisation "Ajout au panier".</t>
   </si>
   <si>
-    <t>Saisit l'adresse de livraison et valide</t>
-  </si>
-  <si>
-    <t>Saisit les informations de paiement et valide</t>
-  </si>
-  <si>
-    <t>Description courte</t>
-  </si>
-  <si>
-    <t>Acteur principal : client
-Acteur secondaire : Banque (système externe à notre périmètre fonctionnelle avec lequel notre système doit communiquer pour la partie paiement)</t>
+    <t>Post-conditions (optionnelles)</t>
+  </si>
+  <si>
+    <t>Pré-condtions (optionnelles)</t>
+  </si>
+  <si>
+    <t>Saisis l'adresse de livraison et valide</t>
+  </si>
+  <si>
+    <t>Saisis les informations de paiement et valide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,7 +242,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -239,28 +252,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -563,9 +579,9 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="B2" s="6"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
@@ -590,13 +606,13 @@
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -624,7 +640,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -647,7 +663,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
@@ -660,24 +676,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="105">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -686,16 +702,16 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -717,8 +733,8 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1"/>
-      <c r="B9" s="7" t="s">
-        <v>28</v>
+      <c r="B9" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -741,8 +757,8 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1"/>
-      <c r="B12" s="7" t="s">
-        <v>29</v>
+      <c r="B12" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -778,7 +794,7 @@
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="30">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -790,7 +806,7 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1"/>
@@ -806,7 +822,7 @@
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">

</xml_diff>